<commit_message>
início das análises para 2023
</commit_message>
<xml_diff>
--- a/dados/csv/2023/4/sint_resumo_por_origem_modalidade_2023.xlsx
+++ b/dados/csv/2023/4/sint_resumo_por_origem_modalidade_2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>origem</t>
   </si>
@@ -43,6 +43,15 @@
     <t>aon_media_sucesso</t>
   </si>
   <si>
+    <t>aon_std_sucesso</t>
+  </si>
+  <si>
+    <t>aon_min_sucesso</t>
+  </si>
+  <si>
+    <t>aon_max_sucesso</t>
+  </si>
+  <si>
     <t>flex</t>
   </si>
   <si>
@@ -64,6 +73,15 @@
     <t>flex_media_sucesso</t>
   </si>
   <si>
+    <t>flex_std_sucesso</t>
+  </si>
+  <si>
+    <t>flex_min_sucesso</t>
+  </si>
+  <si>
+    <t>flex_max_sucesso</t>
+  </si>
+  <si>
     <t>sub</t>
   </si>
   <si>
@@ -83,6 +101,15 @@
   </si>
   <si>
     <t>sub_media_sucesso</t>
+  </si>
+  <si>
+    <t>sub_std_sucesso</t>
+  </si>
+  <si>
+    <t>sub_min_sucesso</t>
+  </si>
+  <si>
+    <t>sub_max_sucesso</t>
   </si>
   <si>
     <t>apoia.se</t>
@@ -452,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,17 +489,23 @@
     <col min="7" max="7" width="9.140625" style="1"/>
     <col min="8" max="8" width="9.140625" style="2"/>
     <col min="9" max="9" width="9.140625" style="2"/>
-    <col min="13" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="9.140625" style="1"/>
-    <col min="15" max="15" width="9.140625" style="2"/>
-    <col min="16" max="16" width="9.140625" style="2"/>
-    <col min="20" max="20" width="9.140625" style="1"/>
-    <col min="21" max="21" width="9.140625" style="1"/>
-    <col min="22" max="22" width="9.140625" style="2"/>
-    <col min="23" max="23" width="9.140625" style="2"/>
+    <col min="10" max="10" width="9.140625" style="2"/>
+    <col min="11" max="11" width="9.140625" style="2"/>
+    <col min="16" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="9.140625" style="1"/>
+    <col min="18" max="18" width="9.140625" style="2"/>
+    <col min="19" max="19" width="9.140625" style="2"/>
+    <col min="20" max="20" width="9.140625" style="2"/>
+    <col min="21" max="21" width="9.140625" style="2"/>
+    <col min="26" max="26" width="9.140625" style="1"/>
+    <col min="27" max="27" width="9.140625" style="1"/>
+    <col min="28" max="28" width="9.140625" style="2"/>
+    <col min="29" max="29" width="9.140625" style="2"/>
+    <col min="30" max="30" width="9.140625" style="2"/>
+    <col min="31" max="31" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:32">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -542,10 +575,37 @@
       <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:32">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>632</v>
@@ -571,52 +631,79 @@
       <c r="I2" s="2">
         <v>0</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
         <v>5</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
         <v>5</v>
       </c>
-      <c r="M2" s="1">
+      <c r="P2" s="1">
         <v>0.003405994550408719</v>
       </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2">
+        <v>0</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
         <v>627</v>
       </c>
-      <c r="R2">
+      <c r="X2">
         <v>137</v>
       </c>
-      <c r="S2">
+      <c r="Y2">
         <v>490</v>
       </c>
-      <c r="T2" s="1">
+      <c r="Z2" s="1">
         <v>0.9166666666666666</v>
       </c>
-      <c r="U2" s="1">
+      <c r="AA2" s="1">
         <v>0.2185007974481659</v>
       </c>
-      <c r="V2" s="2">
+      <c r="AB2" s="2">
         <v>39550.43984210649</v>
       </c>
-      <c r="W2" s="2">
+      <c r="AC2" s="2">
         <v>288.6893419131861</v>
       </c>
+      <c r="AD2" s="2">
+        <v>682.4025885496077</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>1.087396962410123</v>
+      </c>
+      <c r="AF2">
+        <v>5087.076865717208</v>
+      </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:32">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>2855</v>
@@ -642,47 +729,74 @@
       <c r="I3" s="2">
         <v>28991.90340641329</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="2">
+        <v>44961.93536949201</v>
+      </c>
+      <c r="K3" s="2">
+        <v>41.81688448509265</v>
+      </c>
+      <c r="L3">
+        <v>679297.6600721752</v>
+      </c>
+      <c r="M3">
         <v>1463</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>1383</v>
       </c>
-      <c r="L3">
+      <c r="O3">
         <v>80</v>
       </c>
-      <c r="M3" s="1">
+      <c r="P3" s="1">
         <v>0.9965940054495913</v>
       </c>
-      <c r="N3" s="1">
+      <c r="Q3" s="1">
         <v>0.9453178400546821</v>
       </c>
-      <c r="O3" s="2">
+      <c r="R3" s="2">
         <v>18362131.9375591</v>
       </c>
-      <c r="P3" s="2">
+      <c r="S3" s="2">
         <v>13277.02960054888</v>
       </c>
-      <c r="Q3">
+      <c r="T3" s="2">
+        <v>33934.82811955066</v>
+      </c>
+      <c r="U3" s="2">
+        <v>10.77163914429046</v>
+      </c>
+      <c r="V3">
+        <v>708972.7845446636</v>
+      </c>
+      <c r="W3">
         <v>57</v>
       </c>
-      <c r="R3">
+      <c r="X3">
         <v>15</v>
       </c>
-      <c r="S3">
+      <c r="Y3">
         <v>42</v>
       </c>
-      <c r="T3" s="1">
+      <c r="Z3" s="1">
         <v>0.08333333333333333</v>
       </c>
-      <c r="U3" s="1">
+      <c r="AA3" s="1">
         <v>0.2631578947368421</v>
       </c>
-      <c r="V3" s="2">
+      <c r="AB3" s="2">
         <v>3636.517912678314</v>
       </c>
-      <c r="W3" s="2">
+      <c r="AC3" s="2">
         <v>242.4345275118876</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>198.3989605548985</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>10.98162164796783</v>
+      </c>
+      <c r="AF3">
+        <v>538.4389998789497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
análise descritiva do dataset
</commit_message>
<xml_diff>
--- a/dados/csv/2023/4/sint_resumo_por_origem_modalidade_2023.xlsx
+++ b/dados/csv/2023/4/sint_resumo_por_origem_modalidade_2023.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+  <si>
+    <t>geral_modalidade</t>
+  </si>
   <si>
     <t>origem</t>
   </si>
@@ -22,100 +25,46 @@
     <t>total</t>
   </si>
   <si>
+    <t>total_sucesso</t>
+  </si>
+  <si>
+    <t>total_falha</t>
+  </si>
+  <si>
+    <t>particip</t>
+  </si>
+  <si>
+    <t>taxa_sucesso</t>
+  </si>
+  <si>
+    <t>valor_sucesso</t>
+  </si>
+  <si>
+    <t>media_sucesso</t>
+  </si>
+  <si>
+    <t>std_sucesso</t>
+  </si>
+  <si>
+    <t>min_sucesso</t>
+  </si>
+  <si>
+    <t>max_sucesso</t>
+  </si>
+  <si>
     <t>aon</t>
   </si>
   <si>
-    <t>aon_sucesso</t>
-  </si>
-  <si>
-    <t>aon_falha</t>
-  </si>
-  <si>
-    <t>aon_particip</t>
-  </si>
-  <si>
-    <t>aon_taxa_sucesso</t>
-  </si>
-  <si>
-    <t>aon_valor_sucesso</t>
-  </si>
-  <si>
-    <t>aon_media_sucesso</t>
-  </si>
-  <si>
-    <t>aon_std_sucesso</t>
-  </si>
-  <si>
-    <t>aon_min_sucesso</t>
-  </si>
-  <si>
-    <t>aon_max_sucesso</t>
-  </si>
-  <si>
     <t>flex</t>
   </si>
   <si>
-    <t>flex_sucesso</t>
-  </si>
-  <si>
-    <t>flex_falha</t>
-  </si>
-  <si>
-    <t>flex_particip</t>
-  </si>
-  <si>
-    <t>flex_taxa_sucesso</t>
-  </si>
-  <si>
-    <t>flex_valor_sucesso</t>
-  </si>
-  <si>
-    <t>flex_media_sucesso</t>
-  </si>
-  <si>
-    <t>flex_std_sucesso</t>
-  </si>
-  <si>
-    <t>flex_min_sucesso</t>
-  </si>
-  <si>
-    <t>flex_max_sucesso</t>
-  </si>
-  <si>
     <t>sub</t>
   </si>
   <si>
-    <t>sub_sucesso</t>
-  </si>
-  <si>
-    <t>sub_falha</t>
-  </si>
-  <si>
-    <t>sub_particip</t>
-  </si>
-  <si>
-    <t>sub_taxa_sucesso</t>
-  </si>
-  <si>
-    <t>sub_valor_sucesso</t>
-  </si>
-  <si>
-    <t>sub_media_sucesso</t>
-  </si>
-  <si>
-    <t>sub_std_sucesso</t>
-  </si>
-  <si>
-    <t>sub_min_sucesso</t>
-  </si>
-  <si>
-    <t>sub_max_sucesso</t>
+    <t>catarse</t>
   </si>
   <si>
     <t>apoia.se</t>
-  </si>
-  <si>
-    <t>catarse</t>
   </si>
 </sst>
 </file>
@@ -479,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -491,21 +440,10 @@
     <col min="9" max="9" width="9.140625" style="2"/>
     <col min="10" max="10" width="9.140625" style="2"/>
     <col min="11" max="11" width="9.140625" style="2"/>
-    <col min="16" max="16" width="9.140625" style="1"/>
-    <col min="17" max="17" width="9.140625" style="1"/>
-    <col min="18" max="18" width="9.140625" style="2"/>
-    <col min="19" max="19" width="9.140625" style="2"/>
-    <col min="20" max="20" width="9.140625" style="2"/>
-    <col min="21" max="21" width="9.140625" style="2"/>
-    <col min="26" max="26" width="9.140625" style="1"/>
-    <col min="27" max="27" width="9.140625" style="1"/>
-    <col min="28" max="28" width="9.140625" style="2"/>
-    <col min="29" max="29" width="9.140625" style="2"/>
-    <col min="30" max="30" width="9.140625" style="2"/>
-    <col min="31" max="31" width="9.140625" style="2"/>
+    <col min="12" max="12" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:12">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -542,260 +480,194 @@
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>1335</v>
+      </c>
+      <c r="D2">
+        <v>830</v>
+      </c>
+      <c r="E2">
+        <v>505</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.6217228464419475</v>
+      </c>
+      <c r="H2" s="2">
+        <v>24063279.82732303</v>
+      </c>
+      <c r="I2" s="2">
+        <v>28991.90340641329</v>
+      </c>
+      <c r="J2" s="2">
+        <v>44961.93536949201</v>
+      </c>
+      <c r="K2" s="2">
+        <v>41.81688448509265</v>
+      </c>
+      <c r="L2" s="2">
+        <v>679297.6600721752</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.003405994550408719</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>1463</v>
+      </c>
+      <c r="D4">
+        <v>1383</v>
+      </c>
+      <c r="E4">
+        <v>80</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.9965940054495913</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.9453178400546821</v>
+      </c>
+      <c r="H4" s="2">
+        <v>18362131.9375591</v>
+      </c>
+      <c r="I4" s="2">
+        <v>13277.02960054888</v>
+      </c>
+      <c r="J4" s="2">
+        <v>33934.82811955066</v>
+      </c>
+      <c r="K4" s="2">
+        <v>10.77163914429046</v>
+      </c>
+      <c r="L4" s="2">
+        <v>708972.7845446636</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>627</v>
+      </c>
+      <c r="D5">
+        <v>137</v>
+      </c>
+      <c r="E5">
+        <v>490</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.2185007974481659</v>
+      </c>
+      <c r="H5" s="2">
+        <v>39550.43984210649</v>
+      </c>
+      <c r="I5" s="2">
+        <v>288.6893419131861</v>
+      </c>
+      <c r="J5" s="2">
+        <v>682.4025885496077</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1.087396962410123</v>
+      </c>
+      <c r="L5" s="2">
+        <v>5087.076865717208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2">
-        <v>632</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>5</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>5</v>
-      </c>
-      <c r="P2" s="1">
-        <v>0.003405994550408719</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>0</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2">
-        <v>0</v>
-      </c>
-      <c r="U2" s="2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>627</v>
-      </c>
-      <c r="X2">
-        <v>137</v>
-      </c>
-      <c r="Y2">
-        <v>490</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>0.9166666666666666</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>0.2185007974481659</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>39550.43984210649</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>288.6893419131861</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>682.4025885496077</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>1.087396962410123</v>
-      </c>
-      <c r="AF2">
-        <v>5087.076865717208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3">
-        <v>2855</v>
-      </c>
-      <c r="C3">
-        <v>1335</v>
-      </c>
-      <c r="D3">
-        <v>830</v>
-      </c>
-      <c r="E3">
-        <v>505</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.6217228464419475</v>
-      </c>
-      <c r="H3" s="2">
-        <v>24063279.82732303</v>
-      </c>
-      <c r="I3" s="2">
-        <v>28991.90340641329</v>
-      </c>
-      <c r="J3" s="2">
-        <v>44961.93536949201</v>
-      </c>
-      <c r="K3" s="2">
-        <v>41.81688448509265</v>
-      </c>
-      <c r="L3">
-        <v>679297.6600721752</v>
-      </c>
-      <c r="M3">
-        <v>1463</v>
-      </c>
-      <c r="N3">
-        <v>1383</v>
-      </c>
-      <c r="O3">
-        <v>80</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0.9965940054495913</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0.9453178400546821</v>
-      </c>
-      <c r="R3" s="2">
-        <v>18362131.9375591</v>
-      </c>
-      <c r="S3" s="2">
-        <v>13277.02960054888</v>
-      </c>
-      <c r="T3" s="2">
-        <v>33934.82811955066</v>
-      </c>
-      <c r="U3" s="2">
-        <v>10.77163914429046</v>
-      </c>
-      <c r="V3">
-        <v>708972.7845446636</v>
-      </c>
-      <c r="W3">
+      <c r="C6">
         <v>57</v>
       </c>
-      <c r="X3">
+      <c r="D6">
         <v>15</v>
       </c>
-      <c r="Y3">
+      <c r="E6">
         <v>42</v>
       </c>
-      <c r="Z3" s="1">
+      <c r="F6" s="1">
         <v>0.08333333333333333</v>
       </c>
-      <c r="AA3" s="1">
+      <c r="G6" s="1">
         <v>0.2631578947368421</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="H6" s="2">
         <v>3636.517912678314</v>
       </c>
-      <c r="AC3" s="2">
+      <c r="I6" s="2">
         <v>242.4345275118876</v>
       </c>
-      <c r="AD3" s="2">
+      <c r="J6" s="2">
         <v>198.3989605548985</v>
       </c>
-      <c r="AE3" s="2">
+      <c r="K6" s="2">
         <v>10.98162164796783</v>
       </c>
-      <c r="AF3">
+      <c r="L6" s="2">
         <v>538.4389998789497</v>
       </c>
     </row>

</xml_diff>